<commit_message>
added the missing test Wall Clock
</commit_message>
<xml_diff>
--- a/view_results/csvfiles/karthink_profiling_configs.xlsx
+++ b/view_results/csvfiles/karthink_profiling_configs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="34">
   <si>
     <t>#partitions</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Wall Clock</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -474,7 +471,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,8 +744,8 @@
       <c r="G10">
         <v>1000</v>
       </c>
-      <c r="I10" t="s">
-        <v>34</v>
+      <c r="I10">
+        <v>788.13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update loader for histogram
</commit_message>
<xml_diff>
--- a/view_results/csvfiles/karthink_profiling_configs.xlsx
+++ b/view_results/csvfiles/karthink_profiling_configs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Load" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="34">
   <si>
     <t>#partitions</t>
   </si>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1077,7 @@
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1090,8 +1090,11 @@
       <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1133,7 +1136,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1194,6 +1197,28 @@
       </c>
       <c r="C10" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1000</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>